<commit_message>
new documentation and testing
</commit_message>
<xml_diff>
--- a/vignette/Activities/Activity_Patient_X01OV007.xlsx
+++ b/vignette/Activities/Activity_Patient_X01OV007.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E235"/>
+  <dimension ref="A1:E258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4120,11 +4120,6 @@
           <t>ABL1</t>
         </is>
       </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>kin</t>
-        </is>
-      </c>
       <c r="D151">
         <v>2.152359190075838</v>
       </c>
@@ -4145,11 +4140,6 @@
           <t>ACVR2A</t>
         </is>
       </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>kin</t>
-        </is>
-      </c>
       <c r="D152">
         <v>-2.772869360975315</v>
       </c>
@@ -4170,11 +4160,6 @@
           <t>ACVR2B</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>kin</t>
-        </is>
-      </c>
       <c r="D153">
         <v>-3.721045592648255</v>
       </c>
@@ -4195,11 +4180,6 @@
           <t>ALK</t>
         </is>
       </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>kin</t>
-        </is>
-      </c>
       <c r="D154">
         <v>2.872669130928317</v>
       </c>
@@ -4212,21 +4192,16 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Q13315</t>
+          <t>P05089</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>ARG1</t>
         </is>
       </c>
       <c r="D155">
-        <v>-2.782494013537267</v>
+        <v>2.147959809222711</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4237,21 +4212,16 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>P51451</t>
+          <t>Q13315</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>BLK</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>ATM</t>
         </is>
       </c>
       <c r="D156">
-        <v>4.570356478417819</v>
+        <v>-2.782494013537267</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4262,21 +4232,16 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>P36894</t>
+          <t>P51451</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>BMPR1A</t>
-        </is>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>BLK</t>
         </is>
       </c>
       <c r="D157">
-        <v>-6.672588619149533</v>
+        <v>4.570356478417819</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4287,21 +4252,16 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>O00238</t>
+          <t>P36894</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>BMPR1B</t>
-        </is>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>BMPR1A</t>
         </is>
       </c>
       <c r="D158">
-        <v>-6.85770603955863</v>
+        <v>-6.672588619149533</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4312,21 +4272,16 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>P51813</t>
+          <t>O00238</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>BMX</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>BMPR1B</t>
         </is>
       </c>
       <c r="D159">
-        <v>2.603686091630837</v>
+        <v>-6.85770603955863</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4337,21 +4292,16 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Q13554</t>
+          <t>P51813</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>CAMK2B</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>BMX</t>
         </is>
       </c>
       <c r="D160">
-        <v>-3.090244218903302</v>
+        <v>2.603686091630837</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,21 +4312,16 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Q13555</t>
+          <t>Q06187</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>CAMK2G</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>BTK</t>
         </is>
       </c>
       <c r="D161">
-        <v>-3.691091877587153</v>
+        <v>2.705098246959251</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4387,21 +4332,16 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>O00311</t>
+          <t>Q13554</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>CDC7</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>CAMK2B</t>
         </is>
       </c>
       <c r="D162">
-        <v>-3.598217033410549</v>
+        <v>-3.090244218903302</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4412,21 +4352,16 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>P06493</t>
+          <t>Q13555</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>CDK1</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>CAMK2G</t>
         </is>
       </c>
       <c r="D163">
-        <v>-2.069552186879347</v>
+        <v>-3.691091877587153</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4437,21 +4372,16 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>P21709</t>
+          <t>O00311</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>EPHA1</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>CDC7</t>
         </is>
       </c>
       <c r="D164">
-        <v>3.633441446439732</v>
+        <v>-3.598217033410549</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4462,21 +4392,16 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>P29322</t>
+          <t>P06493</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>EPHA8</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>CDK1</t>
         </is>
       </c>
       <c r="D165">
-        <v>4.640954861969721</v>
+        <v>-2.069552186879347</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4487,21 +4412,16 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>P54762</t>
+          <t>P01133</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>EPHB1</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>EGF</t>
         </is>
       </c>
       <c r="D166">
-        <v>2.187207656111925</v>
+        <v>2.209107967266367</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4512,21 +4432,16 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>P54753</t>
+          <t>P21709</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>EPHB3</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>EPHA1</t>
         </is>
       </c>
       <c r="D167">
-        <v>2.288773589560321</v>
+        <v>3.633441446439732</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,21 +4452,16 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>P54760</t>
+          <t>P29322</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>EPHB4</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>EPHA8</t>
         </is>
       </c>
       <c r="D168">
-        <v>3.670788948440323</v>
+        <v>4.640954861969721</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4562,21 +4472,16 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Q8IXL6</t>
+          <t>P54762</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>FAM20C</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>EPHB1</t>
         </is>
       </c>
       <c r="D169">
-        <v>-7.747078084032419</v>
+        <v>2.187207656111925</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,21 +4492,16 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>P16591</t>
+          <t>P54753</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>FER</t>
-        </is>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>EPHB3</t>
         </is>
       </c>
       <c r="D170">
-        <v>2.592010802672276</v>
+        <v>2.288773589560321</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4612,21 +4512,16 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>P06241</t>
+          <t>P54760</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>FYN</t>
-        </is>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>EPHB4</t>
         </is>
       </c>
       <c r="D171">
-        <v>5.858310629235375</v>
+        <v>3.670788948440323</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4637,21 +4532,16 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Q15835</t>
+          <t>Q8IXL6</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>GRK1</t>
-        </is>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>FAM20C</t>
         </is>
       </c>
       <c r="D172">
-        <v>-2.921671531627537</v>
+        <v>-7.747078084032419</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4662,21 +4552,16 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>P25098</t>
+          <t>P16591</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>GRK2</t>
-        </is>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>FER</t>
         </is>
       </c>
       <c r="D173">
-        <v>-2.741785471118299</v>
+        <v>2.592010802672276</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4687,21 +4572,16 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>P35626</t>
+          <t>P06241</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>GRK3</t>
-        </is>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>FYN</t>
         </is>
       </c>
       <c r="D174">
-        <v>-2.782089128984123</v>
+        <v>5.858310629235375</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4712,21 +4592,16 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>P32298</t>
+          <t>Q15835</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>GRK4</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>GRK1</t>
         </is>
       </c>
       <c r="D175">
-        <v>-2.034742052155941</v>
+        <v>-2.921671531627537</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4737,21 +4612,16 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>P34947</t>
+          <t>P25098</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>GRK5</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>GRK2</t>
         </is>
       </c>
       <c r="D176">
-        <v>-1.968106209728591</v>
+        <v>-2.741785471118299</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4762,21 +4632,16 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>P43250</t>
+          <t>P35626</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>GRK6</t>
-        </is>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>GRK3</t>
         </is>
       </c>
       <c r="D177">
-        <v>-3.228082114551379</v>
+        <v>-2.782089128984123</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,21 +4652,16 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>P49840</t>
+          <t>P32298</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>GSK3A</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>GRK4</t>
         </is>
       </c>
       <c r="D178">
-        <v>-3.094670933534459</v>
+        <v>-2.034742052155941</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4812,46 +4672,36 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>P49841</t>
+          <t>P34947</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>GSK3B</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>GRK5</t>
         </is>
       </c>
       <c r="D179">
-        <v>-3.310564506316276</v>
+        <v>-1.968106209728591</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>VIPER+PhosphoScore</t>
+          <t>VIPER</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>P08631</t>
+          <t>P43250</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>HCK</t>
-        </is>
-      </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>GRK6</t>
         </is>
       </c>
       <c r="D180">
-        <v>10.49535571380008</v>
+        <v>-3.228082114551379</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4862,21 +4712,16 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>P51617</t>
+          <t>P49840</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>IRAK1</t>
-        </is>
-      </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>GSK3A</t>
         </is>
       </c>
       <c r="D181">
-        <v>2.061497248320935</v>
+        <v>-3.094670933534459</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4887,12 +4732,12 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Q9NWZ3</t>
+          <t>P49841</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>IRAK4</t>
+          <t>GSK3B</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -4901,32 +4746,27 @@
         </is>
       </c>
       <c r="D182">
-        <v>4.427696687213454</v>
+        <v>-3.310564506316276</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>VIPER</t>
+          <t>VIPER+PhosphoScore</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Q08881</t>
+          <t>P08631</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>ITK</t>
-        </is>
-      </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>HCK</t>
         </is>
       </c>
       <c r="D183">
-        <v>2.751139364759323</v>
+        <v>10.49535571380008</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4937,21 +4777,16 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>P06239</t>
+          <t>P01308</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>LCK</t>
-        </is>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>INS</t>
         </is>
       </c>
       <c r="D184">
-        <v>6.822944143788087</v>
+        <v>3.754978303064354</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4962,21 +4797,16 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Q5S007</t>
+          <t>P51617</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>LRRK2</t>
-        </is>
-      </c>
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>IRAK1</t>
         </is>
       </c>
       <c r="D185">
-        <v>2.538479614537388</v>
+        <v>2.061497248320935</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4987,21 +4817,16 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>P07948</t>
+          <t>Q9NWZ3</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>LYN</t>
-        </is>
-      </c>
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>IRAK4</t>
         </is>
       </c>
       <c r="D186">
-        <v>4.311848112979897</v>
+        <v>4.427696687213454</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,21 +4837,16 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Q6ZN16</t>
+          <t>Q08881</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>MAP3K15</t>
-        </is>
-      </c>
-      <c r="C187" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>ITK</t>
         </is>
       </c>
       <c r="D187">
-        <v>3.057687266652211</v>
+        <v>2.751139364759323</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5037,21 +4857,16 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Q7KZI7</t>
+          <t>P06239</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>MARK2</t>
-        </is>
-      </c>
-      <c r="C188" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>LCK</t>
         </is>
       </c>
       <c r="D188">
-        <v>-2.286879704818966</v>
+        <v>6.822944143788087</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5062,21 +4877,16 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Q12866</t>
+          <t>Q5S007</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>MERTK</t>
-        </is>
-      </c>
-      <c r="C189" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>LRRK2</t>
         </is>
       </c>
       <c r="D189">
-        <v>2.665838788107731</v>
+        <v>2.538479614537388</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5087,21 +4897,16 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>P00540</t>
+          <t>P07948</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>MOS</t>
-        </is>
-      </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>LYN</t>
         </is>
       </c>
       <c r="D190">
-        <v>-2.559954072288121</v>
+        <v>4.311848112979897</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5112,21 +4917,16 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Q8WXR4</t>
+          <t>Q6ZN16</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>MYO3B</t>
-        </is>
-      </c>
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>MAP3K15</t>
         </is>
       </c>
       <c r="D191">
-        <v>2.414169765910408</v>
+        <v>3.057687266652211</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5137,21 +4937,16 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Q96PY6</t>
+          <t>P53779</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>NEK1</t>
-        </is>
-      </c>
-      <c r="C192" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>MAPK10</t>
         </is>
       </c>
       <c r="D192">
-        <v>9.091570298203683</v>
+        <v>-2.275089662915439</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5162,21 +4957,16 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>P51957</t>
+          <t>Q7KZI7</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>NEK4</t>
-        </is>
-      </c>
-      <c r="C193" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>MARK2</t>
         </is>
       </c>
       <c r="D193">
-        <v>2.134097661385318</v>
+        <v>-2.286879704818966</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5187,21 +4977,16 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Q86SG6</t>
+          <t>Q12866</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>NEK8</t>
-        </is>
-      </c>
-      <c r="C194" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>MERTK</t>
         </is>
       </c>
       <c r="D194">
-        <v>6.01977917722416</v>
+        <v>2.665838788107731</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5212,21 +4997,16 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Q9NQU5</t>
+          <t>P00540</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>PAK6</t>
-        </is>
-      </c>
-      <c r="C195" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>MOS</t>
         </is>
       </c>
       <c r="D195">
-        <v>2.011913477103005</v>
+        <v>-2.559954072288121</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5237,21 +5017,16 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Q15118</t>
+          <t>P26927</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>PDK1</t>
-        </is>
-      </c>
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>MST1</t>
         </is>
       </c>
       <c r="D196">
-        <v>2.281792250681337</v>
+        <v>2.103226642502413</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5262,21 +5037,16 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Q16816</t>
+          <t>Q8WXR4</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>PHKG1</t>
-        </is>
-      </c>
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>MYO3B</t>
         </is>
       </c>
       <c r="D197">
-        <v>3.80410077121708</v>
+        <v>2.414169765910408</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5287,21 +5057,16 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>P15735</t>
+          <t>Q96PY6</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>PHKG2</t>
-        </is>
-      </c>
-      <c r="C198" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>NEK1</t>
         </is>
       </c>
       <c r="D198">
-        <v>8.845604731465981</v>
+        <v>9.091570298203683</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5312,21 +5077,16 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Q16512</t>
+          <t>P51957</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>PKN1</t>
-        </is>
-      </c>
-      <c r="C199" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>NEK4</t>
         </is>
       </c>
       <c r="D199">
-        <v>6.563394474151745</v>
+        <v>2.134097661385318</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5337,46 +5097,36 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Q16513</t>
+          <t>Q86SG6</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>PKN2</t>
-        </is>
-      </c>
-      <c r="C200" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>NEK8</t>
         </is>
       </c>
       <c r="D200">
-        <v>0.9750434071471243</v>
+        <v>6.01977917722416</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>VIPER+PhosphoScore</t>
+          <t>VIPER</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Q9NYY3</t>
+          <t>Q9NQU5</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>PLK2</t>
-        </is>
-      </c>
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PAK6</t>
         </is>
       </c>
       <c r="D201">
-        <v>-4.451133342334632</v>
+        <v>2.011913477103005</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5387,21 +5137,16 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Q9H4B4</t>
+          <t>Q15118</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>PLK3</t>
-        </is>
-      </c>
-      <c r="C202" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PDK1</t>
         </is>
       </c>
       <c r="D202">
-        <v>-3.427752725239089</v>
+        <v>2.281792250681337</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5412,21 +5157,16 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>P17252</t>
+          <t>Q16816</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>PRKCA</t>
-        </is>
-      </c>
-      <c r="C203" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PHKG1</t>
         </is>
       </c>
       <c r="D203">
-        <v>7.916686854660441</v>
+        <v>3.80410077121708</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5437,21 +5177,16 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Q14289</t>
+          <t>P15735</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>PTK2B</t>
-        </is>
-      </c>
-      <c r="C204" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PHKG2</t>
         </is>
       </c>
       <c r="D204">
-        <v>6.771109697207317</v>
+        <v>8.845604731465981</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5462,21 +5197,16 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Q13882</t>
+          <t>Q16512</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>PTK6</t>
-        </is>
-      </c>
-      <c r="C205" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PKN1</t>
         </is>
       </c>
       <c r="D205">
-        <v>2.284878422479954</v>
+        <v>6.563394474151745</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5487,12 +5217,12 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>O43353</t>
+          <t>Q16513</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>RIPK2</t>
+          <t>PKN2</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -5501,32 +5231,27 @@
         </is>
       </c>
       <c r="D206">
-        <v>4.8366350701589</v>
+        <v>0.9750434071471243</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>VIPER</t>
+          <t>VIPER+PhosphoScore</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Q13464</t>
+          <t>Q9NYY3</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>ROCK1</t>
-        </is>
-      </c>
-      <c r="C207" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PLK2</t>
         </is>
       </c>
       <c r="D207">
-        <v>5.50694860265276</v>
+        <v>-4.451133342334632</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5537,21 +5262,16 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>P12931</t>
+          <t>Q9H4B4</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>SRC</t>
-        </is>
-      </c>
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PLK3</t>
         </is>
       </c>
       <c r="D208">
-        <v>4.344915259864373</v>
+        <v>-3.427752725239089</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5562,21 +5282,16 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Q9H3Y6</t>
+          <t>P17252</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>SRMS</t>
-        </is>
-      </c>
-      <c r="C209" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PRKCA</t>
         </is>
       </c>
       <c r="D209">
-        <v>3.352118281940172</v>
+        <v>7.916686854660441</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5587,21 +5302,16 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Q9BYT3</t>
+          <t>Q14289</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>STK33</t>
-        </is>
-      </c>
-      <c r="C210" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PTK2B</t>
         </is>
       </c>
       <c r="D210">
-        <v>5.554914234500546</v>
+        <v>6.771109697207317</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5612,21 +5322,16 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>P42680</t>
+          <t>Q13882</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>TEC</t>
-        </is>
-      </c>
-      <c r="C211" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>PTK6</t>
         </is>
       </c>
       <c r="D211">
-        <v>3.861637348499655</v>
+        <v>2.284878422479954</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5637,21 +5342,16 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>P36897</t>
+          <t>O43353</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>TGFBR1</t>
-        </is>
-      </c>
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>RIPK2</t>
         </is>
       </c>
       <c r="D212">
-        <v>-4.388193375030116</v>
+        <v>4.8366350701589</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5662,21 +5362,16 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>P43403</t>
+          <t>Q13464</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>ZAP70</t>
-        </is>
-      </c>
-      <c r="C213" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>ROCK1</t>
         </is>
       </c>
       <c r="D213">
-        <v>3.264655354020482</v>
+        <v>5.50694860265276</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5687,171 +5382,141 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Q9NYV4</t>
+          <t>P12931</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>CDK12</t>
-        </is>
-      </c>
-      <c r="C214" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>SRC</t>
         </is>
       </c>
       <c r="D214">
-        <v>2.731230736166809</v>
+        <v>4.344915259864373</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>PhosphoScore</t>
+          <t>VIPER</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>O96017</t>
+          <t>Q9H3Y6</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>CHEK2</t>
-        </is>
-      </c>
-      <c r="C215" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>SRMS</t>
         </is>
       </c>
       <c r="D215">
-        <v>3.513470046786272</v>
+        <v>3.352118281940172</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>PhosphoScore</t>
+          <t>VIPER</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>P45985</t>
+          <t>Q9BYT3</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>MAP2K4</t>
-        </is>
-      </c>
-      <c r="C216" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>STK33</t>
         </is>
       </c>
       <c r="D216">
-        <v>-2.181006734957414</v>
+        <v>5.554914234500546</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>PhosphoScore</t>
+          <t>VIPER</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>O96013</t>
+          <t>P42680</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>PAK4</t>
-        </is>
-      </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>TEC</t>
         </is>
       </c>
       <c r="D217">
-        <v>2.411415501863389</v>
+        <v>3.861637348499655</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>PhosphoScore</t>
+          <t>VIPER</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Q14738</t>
+          <t>P36897</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>PPP2R5D</t>
-        </is>
-      </c>
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>phos</t>
+          <t>TGFBR1</t>
         </is>
       </c>
       <c r="D218">
-        <v>-2.10544336216922</v>
+        <v>-4.388193375030116</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>PhosphoScore</t>
+          <t>VIPER</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Q05655</t>
+          <t>P43403</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>PRKCD</t>
-        </is>
-      </c>
-      <c r="C219" t="inlineStr">
-        <is>
-          <t>kin</t>
+          <t>ZAP70</t>
         </is>
       </c>
       <c r="D219">
-        <v>2.655305949926098</v>
+        <v>3.264655354020482</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>PhosphoScore</t>
+          <t>VIPER</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Q06124;Q06124</t>
+          <t>Q14155;Q14155</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>PTPN11</t>
+          <t>ARHGEF7</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>phos</t>
+          <t>other</t>
         </is>
       </c>
       <c r="D220">
-        <v>2.021472922934361</v>
+        <v>2.177158465464768</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5862,21 +5527,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>P18433;P18433</t>
+          <t>P17655</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>PTPRA</t>
+          <t>CAPN2</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>phos</t>
+          <t>other</t>
         </is>
       </c>
       <c r="D221">
-        <v>2.215641160391233</v>
+        <v>-3.0815017962367</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5887,12 +5552,12 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>O75385</t>
+          <t>Q9NYV4</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>ULK1</t>
+          <t>CDK12</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -5901,7 +5566,7 @@
         </is>
       </c>
       <c r="D222">
-        <v>-2.160237191433707</v>
+        <v>2.731230736166809</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5912,21 +5577,21 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Q14155;Q14155</t>
+          <t>O96017</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>ARHGEF7</t>
+          <t>CHEK2</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>kin</t>
         </is>
       </c>
       <c r="D223">
-        <v>2.177158465464768</v>
+        <v>3.513470046786272</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5937,12 +5602,12 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>P17655</t>
+          <t>Q99704</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>CAPN2</t>
+          <t>DOK1</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -5951,7 +5616,7 @@
         </is>
       </c>
       <c r="D224">
-        <v>-3.0815017962367</v>
+        <v>1.971031394335562</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5962,21 +5627,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Q99704</t>
+          <t>Q12778</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>DOK1</t>
+          <t>FOXO1</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>tf</t>
         </is>
       </c>
       <c r="D225">
-        <v>1.971031394335562</v>
+        <v>1.988226564625402</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6037,21 +5702,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>P18669</t>
+          <t>P17275</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>PGAM1</t>
+          <t>JUNB</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>tf</t>
         </is>
       </c>
       <c r="D228">
-        <v>-2.753206316848275</v>
+        <v>2.363180868769115</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6062,21 +5727,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Q01970</t>
+          <t>P45985</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>PLCB3</t>
+          <t>MAP2K4</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>kin</t>
         </is>
       </c>
       <c r="D229">
-        <v>-2.127942130475608</v>
+        <v>-2.181006734957414</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6087,21 +5752,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>O60237</t>
+          <t>Q14814</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>PPP1R12B</t>
+          <t>MEF2D</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>tf</t>
         </is>
       </c>
       <c r="D230">
-        <v>-3.253721593203791</v>
+        <v>-2.411870925444964</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6112,21 +5777,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Q15185</t>
+          <t>O96013</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>PTGES3</t>
+          <t>PAK4</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>kin</t>
         </is>
       </c>
       <c r="D231">
-        <v>-3.461518408635544</v>
+        <v>2.411415501863389</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6137,12 +5802,12 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>P49023;P49023</t>
+          <t>P18669</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>PXN</t>
+          <t>PGAM1</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -6151,7 +5816,7 @@
         </is>
       </c>
       <c r="D232">
-        <v>2.276251404900416</v>
+        <v>-2.753206316848275</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6162,12 +5827,12 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>P10301</t>
+          <t>Q01970</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>RRAS</t>
+          <t>PLCB3</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -6176,7 +5841,7 @@
         </is>
       </c>
       <c r="D233">
-        <v>2.438920323711084</v>
+        <v>-2.127942130475608</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6187,12 +5852,12 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Q9Y2K6</t>
+          <t>O60237</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>USP20</t>
+          <t>PPP1R12B</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -6201,7 +5866,7 @@
         </is>
       </c>
       <c r="D234">
-        <v>-2.69763691434521</v>
+        <v>-3.253721593203791</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6212,23 +5877,598 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
+          <t>Q14738</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>PPP2R5D</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>phos</t>
+        </is>
+      </c>
+      <c r="D235">
+        <v>-2.10544336216922</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Q05655</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>PRKCD</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>kin</t>
+        </is>
+      </c>
+      <c r="D236">
+        <v>2.655305949926098</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Q15185</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>PTGES3</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D237">
+        <v>-3.461518408635544</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Q06124;Q06124</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>PTPN11</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>phos</t>
+        </is>
+      </c>
+      <c r="D238">
+        <v>2.021472922934361</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>P18433;P18433</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>PTPRA</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>phos</t>
+        </is>
+      </c>
+      <c r="D239">
+        <v>2.215641160391233</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>P49023;P49023</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>PXN</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D240">
+        <v>2.276251404900416</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>P10301</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>RRAS</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D241">
+        <v>2.438920323711084</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>P19484</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>TFEB</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>tf</t>
+        </is>
+      </c>
+      <c r="D242">
+        <v>2.48458803166739</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>O75385</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>ULK1</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>kin</t>
+        </is>
+      </c>
+      <c r="D243">
+        <v>-2.160237191433707</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Q9Y2K6</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>USP20</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D244">
+        <v>-2.69763691434521</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
           <t>P08670</t>
         </is>
       </c>
-      <c r="B235" t="inlineStr">
+      <c r="B245" t="inlineStr">
         <is>
           <t>VIM</t>
         </is>
       </c>
-      <c r="C235" t="inlineStr">
+      <c r="C245" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="D235">
+      <c r="D245">
         <v>2.023976756175782</v>
       </c>
-      <c r="E235" t="inlineStr">
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Q14155;Q14155</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>ARHGEF7</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D246">
+        <v>2.177158465464768</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>P17655</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>CAPN2</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D247">
+        <v>-3.0815017962367</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Q99704</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>DOK1</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D248">
+        <v>1.971031394335562</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>P42858</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>HTT</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D249">
+        <v>-1.989679255111472</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Q9Y4H2</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>IRS2</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D250">
+        <v>3.011270877995901</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>P18669</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>PGAM1</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D251">
+        <v>-2.753206316848275</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Q01970</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>PLCB3</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D252">
+        <v>-2.127942130475608</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>O60237</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>PPP1R12B</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D253">
+        <v>-3.253721593203791</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Q15185</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>PTGES3</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D254">
+        <v>-3.461518408635544</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>P49023;P49023</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>PXN</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D255">
+        <v>2.276251404900416</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>P10301</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>RRAS</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D256">
+        <v>2.438920323711084</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Q9Y2K6</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>USP20</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D257">
+        <v>-2.69763691434521</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>PhosphoScore</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>P08670</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>VIM</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="D258">
+        <v>2.023976756175782</v>
+      </c>
+      <c r="E258" t="inlineStr">
         <is>
           <t>PhosphoScore</t>
         </is>

</xml_diff>